<commit_message>
ya no se qeu hacer
</commit_message>
<xml_diff>
--- a/my_data.xlsx
+++ b/my_data.xlsx
@@ -1378,7 +1378,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1740,13 +1740,13 @@
     <col min="1" max="1" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="58.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="43.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="213.57642857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="481.14785714285716" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="2" t="s">
         <v>46</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="2" t="s">
         <v>61</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="2" t="s">
         <v>65</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="2" t="s">
         <v>69</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>73</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="2" t="s">
         <v>74</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="2" t="s">
         <v>78</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
       <c r="A18" s="2" t="s">
         <v>82</v>
       </c>

</xml_diff>